<commit_message>
kNN: Learning by one feature
</commit_message>
<xml_diff>
--- a/reports/Report.xlsx
+++ b/reports/Report.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="110">
   <si>
     <t xml:space="preserve">Название метода </t>
   </si>
@@ -172,6 +172,180 @@
   </si>
   <si>
     <t>долго</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 0)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 1)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 2)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 3)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 4)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 5)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 6)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 7)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 8)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 9)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 10)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 11)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 12)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 13)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 14)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 15)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 16)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 17)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 18)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 19)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 20)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 21)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 22)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 23)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 24)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 25)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 26)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 27)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 28)</t>
+  </si>
+  <si>
+    <t>kNN (по столбцу № 29)</t>
+  </si>
+  <si>
+    <t>~0,2</t>
+  </si>
+  <si>
+    <t>~0,3</t>
+  </si>
+  <si>
+    <t>~0,4</t>
+  </si>
+  <si>
+    <t>~0,5</t>
+  </si>
+  <si>
+    <t>~0,6</t>
+  </si>
+  <si>
+    <t>~0,7</t>
+  </si>
+  <si>
+    <t>~0,8</t>
+  </si>
+  <si>
+    <t>~0,9</t>
+  </si>
+  <si>
+    <t>~0,10</t>
+  </si>
+  <si>
+    <t>~0,11</t>
+  </si>
+  <si>
+    <t>~0,12</t>
+  </si>
+  <si>
+    <t>~0,13</t>
+  </si>
+  <si>
+    <t>~0,14</t>
+  </si>
+  <si>
+    <t>~0,15</t>
+  </si>
+  <si>
+    <t>~0,16</t>
+  </si>
+  <si>
+    <t>~0,17</t>
+  </si>
+  <si>
+    <t>~0,18</t>
+  </si>
+  <si>
+    <t>~0,19</t>
+  </si>
+  <si>
+    <t>~0,20</t>
+  </si>
+  <si>
+    <t>~0,21</t>
+  </si>
+  <si>
+    <t>~0,22</t>
+  </si>
+  <si>
+    <t>~0,23</t>
+  </si>
+  <si>
+    <t>~0,24</t>
+  </si>
+  <si>
+    <t>~0,25</t>
+  </si>
+  <si>
+    <t>~0,26</t>
+  </si>
+  <si>
+    <t>~0,27</t>
+  </si>
+  <si>
+    <t>~0,28</t>
+  </si>
+  <si>
+    <t>~0,29</t>
   </si>
 </sst>
 </file>
@@ -333,7 +507,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -513,8 +687,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14996795556505021"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -644,6 +824,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -689,7 +954,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -699,6 +964,39 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -745,9 +1043,216 @@
     <cellStyle name="Текст предупреждения" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Хороший" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:G68" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+  <autoFilter ref="A1:G68"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Название метода " dataDxfId="8"/>
+    <tableColumn id="2" name=" Параметры " dataDxfId="7"/>
+    <tableColumn id="3" name="Объем выборки" dataDxfId="6"/>
+    <tableColumn id="4" name="Метод проверки" dataDxfId="5"/>
+    <tableColumn id="5" name="Точность (матожидание)" dataDxfId="4"/>
+    <tableColumn id="6" name="Доверительный интервал (+/-) p=0,05" dataDxfId="3"/>
+    <tableColumn id="7" name="Время работы (сек)" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1035,42 +1540,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.85546875" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="4" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="26.5703125" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="6" max="6" width="37.7109375" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.5" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
@@ -1078,168 +1584,168 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2">
-        <v>5000</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="C2" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="11">
         <v>0.73</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="11">
         <v>0.02</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="12">
         <v>2622.81</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2">
-        <v>5000</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="C3" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="11">
         <v>0.78</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="11">
         <v>0.02</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="12">
         <v>10.199999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G4" s="5">
+        <v>6.87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G5" s="5">
+        <v>4.8099999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B6" s="11">
         <v>5</v>
       </c>
-      <c r="C4" s="2">
-        <v>5000</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="C6" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="11">
         <v>0.76</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F6" s="11">
         <v>0.02</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G6" s="12">
         <v>0.49</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="2" t="s">
+    <row r="7" spans="1:9">
+      <c r="A7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2">
-        <v>5000</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="B7" s="11">
+        <v>12</v>
+      </c>
+      <c r="C7" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="11">
         <v>0.78</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F7" s="11">
         <v>0.02</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G7" s="12">
         <v>0.65</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2">
-        <v>5000</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.74</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="G6" s="2">
-        <v>6.87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="2">
-        <v>5000</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.66</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="G7" s="2">
-        <v>4.8099999999999996</v>
-      </c>
-    </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="2">
-        <v>5000</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="C8" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="11">
         <v>0.76</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="11">
         <v>0.03</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="12">
         <v>0.63</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1257,12 +1763,12 @@
       <c r="F9" s="2">
         <v>0.01</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="5">
         <v>1874.2</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1280,12 +1786,12 @@
       <c r="F10" s="2">
         <v>0.01</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="5">
         <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1299,12 +1805,12 @@
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1322,12 +1828,12 @@
       <c r="F12" s="2">
         <v>0.01</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="5">
         <v>3436.85</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1345,12 +1851,12 @@
       <c r="F13" s="2">
         <v>0.01</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="5">
         <v>1.98</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1368,12 +1874,12 @@
       <c r="F14" s="2">
         <v>0.02</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="5">
         <v>23805.64</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1391,12 +1897,12 @@
       <c r="F15" s="2">
         <v>0.01</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="5">
         <v>99.05</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1414,12 +1920,12 @@
       <c r="F16" s="2">
         <v>0.01</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="5">
         <v>1.37</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1437,12 +1943,12 @@
       <c r="F17" s="2">
         <v>0.01</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1460,12 +1966,12 @@
       <c r="F18" s="2">
         <v>0.01</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="5">
         <v>2076.38</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1483,12 +1989,12 @@
       <c r="F19" s="2">
         <v>0.01</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="5">
         <v>1.5</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1506,12 +2012,12 @@
       <c r="F20" s="2">
         <v>0.01</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="5">
         <v>1.45</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1529,12 +2035,12 @@
       <c r="F21" s="2">
         <v>0.01</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="5">
         <v>1.29</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1552,12 +2058,12 @@
       <c r="F22" s="2">
         <v>0.02</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="5">
         <v>37.479999999999997</v>
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1575,12 +2081,12 @@
       <c r="F23" s="2">
         <v>0.01</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="5">
         <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1598,12 +2104,12 @@
       <c r="F24" s="2">
         <v>0.01</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="5">
         <v>1.23</v>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1621,12 +2127,12 @@
       <c r="F25" s="2">
         <v>0.01</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="5">
         <v>1494.93</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1644,12 +2150,12 @@
       <c r="F26" s="2">
         <v>0.01</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="5">
         <v>1.29</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1667,12 +2173,12 @@
       <c r="F27" s="2">
         <v>0.01</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="5">
         <v>1.17</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1686,12 +2192,12 @@
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1705,12 +2211,12 @@
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -1722,12 +2228,18 @@
       <c r="D30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+      <c r="E30" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F30" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G30" s="5">
+        <v>2760.94</v>
+      </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -1739,12 +2251,18 @@
       <c r="D31" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
+      <c r="E31" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G31" s="5">
+        <v>1.04</v>
+      </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1756,12 +2274,18 @@
       <c r="D32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="E32" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G32" s="5">
+        <v>4896.7700000000004</v>
+      </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -1773,12 +2297,18 @@
       <c r="D33" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
+      <c r="E33" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G33" s="5">
+        <v>1.56</v>
+      </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1790,12 +2320,18 @@
       <c r="D34" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="E34" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G34" s="5">
+        <v>1.44</v>
+      </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="4" t="s">
         <v>46</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1807,12 +2343,18 @@
       <c r="D35" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
+      <c r="E35" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G35" s="5">
+        <v>3678.42</v>
+      </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -1824,12 +2366,18 @@
       <c r="D36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
+      <c r="E36" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G36" s="5">
+        <v>1.38</v>
+      </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -1841,12 +2389,18 @@
       <c r="D37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
+      <c r="E37" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G37" s="5">
+        <v>1.1000000000000001</v>
+      </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -1860,11 +2414,706 @@
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+      <c r="G38" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="11">
+        <v>12</v>
+      </c>
+      <c r="C39" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="11">
+        <v>0.72</v>
+      </c>
+      <c r="F39" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="G39" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="11">
+        <v>12</v>
+      </c>
+      <c r="C40" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="11">
+        <v>0.67</v>
+      </c>
+      <c r="F40" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" s="11">
+        <v>12</v>
+      </c>
+      <c r="C41" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="11">
+        <v>0.66</v>
+      </c>
+      <c r="F41" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" s="11">
+        <v>12</v>
+      </c>
+      <c r="C42" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="11">
+        <v>0.66</v>
+      </c>
+      <c r="F42" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" s="11">
+        <v>12</v>
+      </c>
+      <c r="C43" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="11">
+        <v>0.69</v>
+      </c>
+      <c r="F43" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="G43" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="11">
+        <v>12</v>
+      </c>
+      <c r="C44" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="11">
+        <v>0.68</v>
+      </c>
+      <c r="F44" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" s="11">
+        <v>12</v>
+      </c>
+      <c r="C45" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="11">
+        <v>0.68</v>
+      </c>
+      <c r="F45" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="G45" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" s="11">
+        <v>12</v>
+      </c>
+      <c r="C46" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="11">
+        <v>0.63</v>
+      </c>
+      <c r="F46" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47" s="11">
+        <v>12</v>
+      </c>
+      <c r="C47" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="11">
+        <v>0.63</v>
+      </c>
+      <c r="F47" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48" s="11">
+        <v>12</v>
+      </c>
+      <c r="C48" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="11">
+        <v>0.64</v>
+      </c>
+      <c r="F48" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B49" s="11">
+        <v>12</v>
+      </c>
+      <c r="C49" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="11">
+        <v>0.68</v>
+      </c>
+      <c r="F49" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" s="11">
+        <v>12</v>
+      </c>
+      <c r="C50" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="11">
+        <v>0.66</v>
+      </c>
+      <c r="F50" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="G50" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" s="11">
+        <v>12</v>
+      </c>
+      <c r="C51" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="11">
+        <v>0.66</v>
+      </c>
+      <c r="F51" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" s="11">
+        <v>12</v>
+      </c>
+      <c r="C52" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="11">
+        <v>0.66</v>
+      </c>
+      <c r="F52" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" s="11">
+        <v>12</v>
+      </c>
+      <c r="C53" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="11">
+        <v>0.63</v>
+      </c>
+      <c r="F53" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="G53" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="11">
+        <v>12</v>
+      </c>
+      <c r="C54" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="11">
+        <v>0.64</v>
+      </c>
+      <c r="F54" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="G54" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" s="11">
+        <v>12</v>
+      </c>
+      <c r="C55" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="11">
+        <v>0.63</v>
+      </c>
+      <c r="F55" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="G55" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B56" s="11">
+        <v>12</v>
+      </c>
+      <c r="C56" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="11">
+        <v>0.64</v>
+      </c>
+      <c r="F56" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B57" s="11">
+        <v>12</v>
+      </c>
+      <c r="C57" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="11">
+        <v>0.64</v>
+      </c>
+      <c r="F57" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="G57" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58" s="11">
+        <v>12</v>
+      </c>
+      <c r="C58" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="11">
+        <v>0.64</v>
+      </c>
+      <c r="F58" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="G58" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B59" s="11">
+        <v>12</v>
+      </c>
+      <c r="C59" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="11">
+        <v>0.62</v>
+      </c>
+      <c r="F59" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B60" s="11">
+        <v>12</v>
+      </c>
+      <c r="C60" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="11">
+        <v>0.62</v>
+      </c>
+      <c r="F60" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="G60" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B61" s="11">
+        <v>12</v>
+      </c>
+      <c r="C61" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="11">
+        <v>0.66</v>
+      </c>
+      <c r="F61" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="G61" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B62" s="11">
+        <v>12</v>
+      </c>
+      <c r="C62" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="11">
+        <v>0.63</v>
+      </c>
+      <c r="F62" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="G62" s="12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B63" s="11">
+        <v>12</v>
+      </c>
+      <c r="C63" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="11">
+        <v>0.64</v>
+      </c>
+      <c r="F63" s="11">
+        <v>0.03</v>
+      </c>
+      <c r="G63" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B64" s="11">
+        <v>12</v>
+      </c>
+      <c r="C64" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="11">
+        <v>0.64</v>
+      </c>
+      <c r="F64" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B65" s="11">
+        <v>12</v>
+      </c>
+      <c r="C65" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="11">
+        <v>0.59</v>
+      </c>
+      <c r="F65" s="11">
+        <v>0.24</v>
+      </c>
+      <c r="G65" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B66" s="11">
+        <v>12</v>
+      </c>
+      <c r="C66" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D66" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" s="11">
+        <v>0.66</v>
+      </c>
+      <c r="F66" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="G66" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B67" s="11">
+        <v>12</v>
+      </c>
+      <c r="C67" s="11">
+        <v>5000</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="11">
+        <v>0.65</v>
+      </c>
+      <c r="F67" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="G67" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B68" s="11">
+        <v>12</v>
+      </c>
+      <c r="C68" s="14">
+        <v>5000</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="14">
+        <v>0.65</v>
+      </c>
+      <c r="F68" s="14">
+        <v>0.02</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>109</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>